<commit_message>
fix weird encoded chars
</commit_message>
<xml_diff>
--- a/Raw Input Data/Processing/Case 46/Suspect transaction.xlsx
+++ b/Raw Input Data/Processing/Case 46/Suspect transaction.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hbap.adroot.hsbc\HK\HASE\28062201\Fraud_Ops_FIM_File_Sharing\HASE case\Gen AI\Upload to sharepoint\Batch 5\Case 46 (UAR)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Processing\Case 46\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B2F7FE-E165-4982-B8B9-70A1A0922D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23258" windowHeight="14018"/>
+    <workbookView xWindow="-25290" yWindow="6810" windowWidth="20520" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaction record" sheetId="2" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Transaction Date (value)</t>
   </si>
@@ -124,18 +114,6 @@
     <t>ATM/CDM CASH CREDIT USINGACCOUNT INPUT</t>
   </si>
   <si>
-    <t>１＝３</t>
-  </si>
-  <si>
-    <t>２＝４</t>
-  </si>
-  <si>
-    <t>５</t>
-  </si>
-  <si>
-    <t>６</t>
-  </si>
-  <si>
     <t xml:space="preserve">CHAN TAI MAN </t>
   </si>
   <si>
@@ -149,16 +127,22 @@
   </si>
   <si>
     <t>COUNTERPARTY_NOT_STATED –111-111111-101 - CASH TXN CREDIT</t>
+  </si>
+  <si>
+    <t>1=3</t>
+  </si>
+  <si>
+    <t>2=4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,23 +220,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,35 +570,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.125" customWidth="1"/>
-    <col min="9" max="9" width="44.3125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.1875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.6875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13.9">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,245 +647,223 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="13.9">
-      <c r="A2" s="7">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>45674</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="3">
+        <v>200000</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>45674</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4000</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="3">
+        <v>4000</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>45675</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="3">
+        <v>100000</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>45676</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22000</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4">
-        <v>200000</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="4">
-        <v>200000</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>29</v>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3">
+        <v>22000</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="13.9">
-      <c r="A3" s="7">
-        <v>45674</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4">
-        <v>4000</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="4">
-        <v>4000</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>30</v>
-      </c>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="Q6" s="5"/>
     </row>
-    <row r="4" spans="1:17" ht="13.9">
-      <c r="A4" s="7">
-        <v>45675</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4">
-        <v>100000</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" s="4">
-        <v>100000</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="7">
-        <v>45676</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="4">
-        <v>22000</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4">
-        <v>22000</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="14.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" ht="14.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="6"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="Q7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -913,6 +875,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002A8F4FDE63F23240996C0B5ED71CAB02" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61b2ee7a38442529347de99e33b69841">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc14db02-3d39-436b-9056-63d1dbe054e8" xmlns:ns3="5ed3fcfa-dd51-4f96-90c6-6669337cd654" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="405649729e347460199c909c216f19f3" ns2:_="" ns3:_="">
     <xsd:import namespace="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
@@ -1107,34 +1089,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5ed3fcfa-dd51-4f96-90c6-6669337cd654" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fc14db02-3d39-436b-9056-63d1dbe054e8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CE89C3-3402-4BCD-841B-432DC7C34F3C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F689B-460C-4633-9D87-3B10FC603704}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAB59A2-24F1-4130-A482-5E26283AC2C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CAB59A2-24F1-4130-A482-5E26283AC2C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F689B-460C-4633-9D87-3B10FC603704}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5CE89C3-3402-4BCD-841B-432DC7C34F3C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc14db02-3d39-436b-9056-63d1dbe054e8"/>
+    <ds:schemaRef ds:uri="5ed3fcfa-dd51-4f96-90c6-6669337cd654"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>